<commit_message>
added new data correction methods
</commit_message>
<xml_diff>
--- a/Duplicated Values.xlsx
+++ b/Duplicated Values.xlsx
@@ -16,426 +16,429 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="140">
-  <si>
-    <t>Values</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="762" uniqueCount="141">
+  <si>
+    <t>Water_Level</t>
   </si>
   <si>
     <t>Timestamp</t>
   </si>
   <si>
-    <t>2020/10/1 0</t>
-  </si>
-  <si>
-    <t>2020/10/1 1</t>
-  </si>
-  <si>
-    <t>2020/10/1 10</t>
-  </si>
-  <si>
-    <t>2020/10/1 11</t>
-  </si>
-  <si>
-    <t>2020/10/1 12</t>
-  </si>
-  <si>
-    <t>2020/10/1 13</t>
-  </si>
-  <si>
-    <t>2020/10/1 14</t>
-  </si>
-  <si>
-    <t>2020/10/1 2</t>
-  </si>
-  <si>
-    <t>2020/10/1 3</t>
-  </si>
-  <si>
-    <t>2020/10/1 4</t>
-  </si>
-  <si>
-    <t>2020/10/1 5</t>
-  </si>
-  <si>
-    <t>2020/10/1 6</t>
-  </si>
-  <si>
-    <t>2020/10/1 7</t>
-  </si>
-  <si>
-    <t>2020/10/1 8</t>
-  </si>
-  <si>
-    <t>2020/10/1 9</t>
-  </si>
-  <si>
-    <t>2020/4/29 0</t>
-  </si>
-  <si>
-    <t>2020/4/29 1</t>
-  </si>
-  <si>
-    <t>2020/4/29 2</t>
-  </si>
-  <si>
-    <t>2020/4/29 3</t>
-  </si>
-  <si>
-    <t>2020/4/29 4</t>
-  </si>
-  <si>
-    <t>2020/4/29 5</t>
-  </si>
-  <si>
-    <t>2020/4/29 6</t>
-  </si>
-  <si>
-    <t>2020/4/29 7</t>
-  </si>
-  <si>
-    <t>2020/4/29 8</t>
-  </si>
-  <si>
-    <t>2020/4/29 9</t>
-  </si>
-  <si>
-    <t>2020/5/19 0</t>
-  </si>
-  <si>
-    <t>2020/5/19 1</t>
-  </si>
-  <si>
-    <t>2020/5/19 10</t>
-  </si>
-  <si>
-    <t>2020/5/19 2</t>
-  </si>
-  <si>
-    <t>2020/5/19 3</t>
-  </si>
-  <si>
-    <t>2020/5/19 4</t>
-  </si>
-  <si>
-    <t>2020/5/19 5</t>
-  </si>
-  <si>
-    <t>2020/5/19 6</t>
-  </si>
-  <si>
-    <t>2020/5/19 7</t>
-  </si>
-  <si>
-    <t>2020/5/19 8</t>
-  </si>
-  <si>
-    <t>2020/5/19 9</t>
-  </si>
-  <si>
-    <t>2020/6/23 0</t>
-  </si>
-  <si>
-    <t>2020/6/23 1</t>
-  </si>
-  <si>
-    <t>2020/6/23 10</t>
-  </si>
-  <si>
-    <t>2020/6/23 11</t>
-  </si>
-  <si>
-    <t>2020/6/23 12</t>
-  </si>
-  <si>
-    <t>2020/6/23 13</t>
-  </si>
-  <si>
-    <t>2020/6/23 14</t>
-  </si>
-  <si>
-    <t>2020/6/23 2</t>
-  </si>
-  <si>
-    <t>2020/6/23 3</t>
-  </si>
-  <si>
-    <t>2020/6/23 4</t>
-  </si>
-  <si>
-    <t>2020/6/23 5</t>
-  </si>
-  <si>
-    <t>2020/6/23 6</t>
-  </si>
-  <si>
-    <t>2020/6/23 7</t>
-  </si>
-  <si>
-    <t>2020/6/23 8</t>
-  </si>
-  <si>
-    <t>2020/6/23 9</t>
-  </si>
-  <si>
-    <t>2020/6/4 0</t>
-  </si>
-  <si>
-    <t>2020/6/4 1</t>
-  </si>
-  <si>
-    <t>2020/6/4 10</t>
-  </si>
-  <si>
-    <t>2020/6/4 11</t>
-  </si>
-  <si>
-    <t>2020/6/4 2</t>
-  </si>
-  <si>
-    <t>2020/6/4 3</t>
-  </si>
-  <si>
-    <t>2020/6/4 4</t>
-  </si>
-  <si>
-    <t>2020/6/4 5</t>
-  </si>
-  <si>
-    <t>2020/6/4 6</t>
-  </si>
-  <si>
-    <t>2020/6/4 7</t>
-  </si>
-  <si>
-    <t>2020/6/4 8</t>
-  </si>
-  <si>
-    <t>2020/6/4 9</t>
-  </si>
-  <si>
-    <t>2020/7/6 0</t>
-  </si>
-  <si>
-    <t>2020/7/6 1</t>
-  </si>
-  <si>
-    <t>2020/7/6 2</t>
-  </si>
-  <si>
-    <t>2020/7/6 3</t>
-  </si>
-  <si>
-    <t>2020/7/6 4</t>
-  </si>
-  <si>
-    <t>2020/7/6 5</t>
-  </si>
-  <si>
-    <t>2020/7/6 6</t>
-  </si>
-  <si>
-    <t>2020/7/6 7</t>
-  </si>
-  <si>
-    <t>2020/7/6 8</t>
-  </si>
-  <si>
-    <t>2020/8/7 0</t>
-  </si>
-  <si>
-    <t>2020/8/7 1</t>
-  </si>
-  <si>
-    <t>2020/8/7 10</t>
-  </si>
-  <si>
-    <t>2020/8/7 11</t>
-  </si>
-  <si>
-    <t>2020/8/7 12</t>
-  </si>
-  <si>
-    <t>2020/8/7 13</t>
-  </si>
-  <si>
-    <t>2020/8/7 14</t>
-  </si>
-  <si>
-    <t>2020/8/7 15</t>
-  </si>
-  <si>
-    <t>2020/8/7 16</t>
-  </si>
-  <si>
-    <t>2020/8/7 2</t>
-  </si>
-  <si>
-    <t>2020/8/7 3</t>
-  </si>
-  <si>
-    <t>2020/8/7 4</t>
-  </si>
-  <si>
-    <t>2020/8/7 5</t>
-  </si>
-  <si>
-    <t>2020/8/7 6</t>
-  </si>
-  <si>
-    <t>2020/8/7 7</t>
-  </si>
-  <si>
-    <t>2020/8/7 8</t>
-  </si>
-  <si>
-    <t>2020/8/7 9</t>
-  </si>
-  <si>
-    <t>2020/9/2 0</t>
-  </si>
-  <si>
-    <t>2020/9/2 1</t>
-  </si>
-  <si>
-    <t>2020/9/2 10</t>
-  </si>
-  <si>
-    <t>2020/9/2 2</t>
-  </si>
-  <si>
-    <t>2020/9/2 3</t>
-  </si>
-  <si>
-    <t>2020/9/2 4</t>
-  </si>
-  <si>
-    <t>2020/9/2 5</t>
-  </si>
-  <si>
-    <t>2020/9/2 6</t>
-  </si>
-  <si>
-    <t>2020/9/2 7</t>
-  </si>
-  <si>
-    <t>2020/9/2 8</t>
-  </si>
-  <si>
-    <t>2020/9/2 9</t>
-  </si>
-  <si>
-    <t>2021/1/1 0</t>
-  </si>
-  <si>
-    <t>2021/1/1 1</t>
-  </si>
-  <si>
-    <t>2021/1/1 10</t>
-  </si>
-  <si>
-    <t>2021/1/1 11</t>
-  </si>
-  <si>
-    <t>2021/1/1 12</t>
-  </si>
-  <si>
-    <t>2021/1/1 13</t>
-  </si>
-  <si>
-    <t>2021/1/1 14</t>
-  </si>
-  <si>
-    <t>2021/1/1 15</t>
-  </si>
-  <si>
-    <t>2021/1/1 16</t>
-  </si>
-  <si>
-    <t>2021/1/1 2</t>
-  </si>
-  <si>
-    <t>2021/1/1 3</t>
-  </si>
-  <si>
-    <t>2021/1/1 4</t>
-  </si>
-  <si>
-    <t>2021/1/1 5</t>
-  </si>
-  <si>
-    <t>2021/1/1 6</t>
-  </si>
-  <si>
-    <t>2021/1/1 7</t>
-  </si>
-  <si>
-    <t>2021/1/1 8</t>
-  </si>
-  <si>
-    <t>2021/1/1 9</t>
-  </si>
-  <si>
-    <t>2021/4/1 0</t>
-  </si>
-  <si>
-    <t>2021/4/1 1</t>
-  </si>
-  <si>
-    <t>2021/4/1 10</t>
-  </si>
-  <si>
-    <t>2021/4/1 2</t>
-  </si>
-  <si>
-    <t>2021/4/1 3</t>
-  </si>
-  <si>
-    <t>2021/4/1 4</t>
-  </si>
-  <si>
-    <t>2021/4/1 5</t>
-  </si>
-  <si>
-    <t>2021/4/1 6</t>
-  </si>
-  <si>
-    <t>2021/4/1 7</t>
-  </si>
-  <si>
-    <t>2021/4/1 8</t>
-  </si>
-  <si>
-    <t>2021/4/1 9</t>
-  </si>
-  <si>
-    <t>2020/5/20 0</t>
-  </si>
-  <si>
-    <t>2020/5/20 1</t>
-  </si>
-  <si>
-    <t>2020/5/20 2</t>
-  </si>
-  <si>
-    <t>2020/5/20 3</t>
-  </si>
-  <si>
-    <t>2020/5/20 4</t>
-  </si>
-  <si>
-    <t>2020/5/20 5</t>
-  </si>
-  <si>
-    <t>2020/5/20 6</t>
-  </si>
-  <si>
-    <t>2020/5/20 7</t>
-  </si>
-  <si>
-    <t>2020/5/20 8</t>
-  </si>
-  <si>
-    <t>2020/5/20 9</t>
+    <t>2020/10/1 0:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 10:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 11:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 12:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 13:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 14:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 1:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 2:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 3:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 4:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 5:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 6:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 7:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 8:00:00</t>
+  </si>
+  <si>
+    <t>2020/10/1 9:00:00</t>
+  </si>
+  <si>
+    <t>2020/4/29 0:00:00</t>
+  </si>
+  <si>
+    <t>2020/4/29 1:00:00</t>
+  </si>
+  <si>
+    <t>2020/4/29 2:00:00</t>
+  </si>
+  <si>
+    <t>2020/4/29 3:00:00</t>
+  </si>
+  <si>
+    <t>2020/4/29 4:00:00</t>
+  </si>
+  <si>
+    <t>2020/4/29 5:00:00</t>
+  </si>
+  <si>
+    <t>2020/4/29 6:00:00</t>
+  </si>
+  <si>
+    <t>2020/4/29 7:00:00</t>
+  </si>
+  <si>
+    <t>2020/4/29 8:00:00</t>
+  </si>
+  <si>
+    <t>2020/4/29 9:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/19 0:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/19 10:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/19 1:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/19 2:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/19 3:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/19 4:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/19 5:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/19 6:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/19 7:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/19 8:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/19 9:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 0:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 10:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 11:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 12:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 13:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 14:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 1:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 2:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 3:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 4:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 5:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 6:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 7:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 8:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/23 9:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/4 0:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/4 10:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/4 11:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/4 1:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/4 2:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/4 3:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/4 4:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/4 5:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/4 6:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/4 7:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/4 8:00:00</t>
+  </si>
+  <si>
+    <t>2020/6/4 9:00:00</t>
+  </si>
+  <si>
+    <t>2020/7/6 0:00:00</t>
+  </si>
+  <si>
+    <t>2020/7/6 1:00:00</t>
+  </si>
+  <si>
+    <t>2020/7/6 2:00:00</t>
+  </si>
+  <si>
+    <t>2020/7/6 3:00:00</t>
+  </si>
+  <si>
+    <t>2020/7/6 4:00:00</t>
+  </si>
+  <si>
+    <t>2020/7/6 5:00:00</t>
+  </si>
+  <si>
+    <t>2020/7/6 6:00:00</t>
+  </si>
+  <si>
+    <t>2020/7/6 7:00:00</t>
+  </si>
+  <si>
+    <t>2020/7/6 8:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 0:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 10:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 11:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 12:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 13:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 14:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 15:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 16:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 1:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 2:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 3:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 4:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 5:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 6:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 7:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 8:00:00</t>
+  </si>
+  <si>
+    <t>2020/8/7 9:00:00</t>
+  </si>
+  <si>
+    <t>2020/9/2 0:00:00</t>
+  </si>
+  <si>
+    <t>2020/9/2 10:00:00</t>
+  </si>
+  <si>
+    <t>2020/9/2 1:00:00</t>
+  </si>
+  <si>
+    <t>2020/9/2 2:00:00</t>
+  </si>
+  <si>
+    <t>2020/9/2 3:00:00</t>
+  </si>
+  <si>
+    <t>2020/9/2 4:00:00</t>
+  </si>
+  <si>
+    <t>2020/9/2 5:00:00</t>
+  </si>
+  <si>
+    <t>2020/9/2 6:00:00</t>
+  </si>
+  <si>
+    <t>2020/9/2 7:00:00</t>
+  </si>
+  <si>
+    <t>2020/9/2 8:00:00</t>
+  </si>
+  <si>
+    <t>2020/9/2 9:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 0:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 10:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 11:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 12:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 13:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 14:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 15:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 16:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 1:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 2:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 3:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 4:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 5:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 6:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 7:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 8:00:00</t>
+  </si>
+  <si>
+    <t>2021/1/1 9:00:00</t>
+  </si>
+  <si>
+    <t>2021/4/1 0:00:00</t>
+  </si>
+  <si>
+    <t>2021/4/1 10:00:00</t>
+  </si>
+  <si>
+    <t>2021/4/1 1:00:00</t>
+  </si>
+  <si>
+    <t>2021/4/1 2:00:00</t>
+  </si>
+  <si>
+    <t>2021/4/1 3:00:00</t>
+  </si>
+  <si>
+    <t>2021/4/1 4:00:00</t>
+  </si>
+  <si>
+    <t>2021/4/1 5:00:00</t>
+  </si>
+  <si>
+    <t>2021/4/1 6:00:00</t>
+  </si>
+  <si>
+    <t>2021/4/1 7:00:00</t>
+  </si>
+  <si>
+    <t>2021/4/1 8:00:00</t>
+  </si>
+  <si>
+    <t>2021/4/1 9:00:00</t>
+  </si>
+  <si>
+    <t>RG0_Level</t>
+  </si>
+  <si>
+    <t>2020/5/20 0:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/20 1:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/20 2:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/20 3:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/20 4:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/20 5:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/20 6:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/20 7:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/20 8:00:00</t>
+  </si>
+  <si>
+    <t>2020/5/20 9:00:00</t>
   </si>
 </sst>
 </file>
@@ -828,7 +831,7 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>2.275565</v>
+        <v>2.227815</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -836,7 +839,7 @@
         <v>3</v>
       </c>
       <c r="B5">
-        <v>2.275565</v>
+        <v>2.227815</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -844,7 +847,7 @@
         <v>4</v>
       </c>
       <c r="B6">
-        <v>2.227815</v>
+        <v>2.15619</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -852,7 +855,7 @@
         <v>4</v>
       </c>
       <c r="B7">
-        <v>2.227815</v>
+        <v>2.15619</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -860,7 +863,7 @@
         <v>5</v>
       </c>
       <c r="B8">
-        <v>2.15619</v>
+        <v>2.227815</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -868,7 +871,7 @@
         <v>5</v>
       </c>
       <c r="B9">
-        <v>2.15619</v>
+        <v>2.227815</v>
       </c>
     </row>
     <row r="10" spans="1:2">
@@ -876,7 +879,7 @@
         <v>6</v>
       </c>
       <c r="B10">
-        <v>2.227815</v>
+        <v>2.20394</v>
       </c>
     </row>
     <row r="11" spans="1:2">
@@ -884,7 +887,7 @@
         <v>6</v>
       </c>
       <c r="B11">
-        <v>2.227815</v>
+        <v>2.20394</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -892,7 +895,7 @@
         <v>7</v>
       </c>
       <c r="B12">
-        <v>2.20394</v>
+        <v>2.084565</v>
       </c>
     </row>
     <row r="13" spans="1:2">
@@ -900,7 +903,7 @@
         <v>7</v>
       </c>
       <c r="B13">
-        <v>2.20394</v>
+        <v>2.084565</v>
       </c>
     </row>
     <row r="14" spans="1:2">
@@ -908,7 +911,7 @@
         <v>8</v>
       </c>
       <c r="B14">
-        <v>2.084565</v>
+        <v>2.275565</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -916,7 +919,7 @@
         <v>8</v>
       </c>
       <c r="B15">
-        <v>2.084565</v>
+        <v>2.275565</v>
       </c>
     </row>
     <row r="16" spans="1:2">
@@ -1404,7 +1407,7 @@
         <v>39</v>
       </c>
       <c r="B76">
-        <v>2.10844</v>
+        <v>1.893565</v>
       </c>
     </row>
     <row r="77" spans="1:2">
@@ -1412,7 +1415,7 @@
         <v>39</v>
       </c>
       <c r="B77">
-        <v>2.10844</v>
+        <v>1.893565</v>
       </c>
     </row>
     <row r="78" spans="1:2">
@@ -1420,7 +1423,7 @@
         <v>40</v>
       </c>
       <c r="B78">
-        <v>1.893565</v>
+        <v>1.91744</v>
       </c>
     </row>
     <row r="79" spans="1:2">
@@ -1428,7 +1431,7 @@
         <v>40</v>
       </c>
       <c r="B79">
-        <v>1.893565</v>
+        <v>1.91744</v>
       </c>
     </row>
     <row r="80" spans="1:2">
@@ -1436,7 +1439,7 @@
         <v>41</v>
       </c>
       <c r="B80">
-        <v>1.91744</v>
+        <v>1.86969</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -1444,7 +1447,7 @@
         <v>41</v>
       </c>
       <c r="B81">
-        <v>1.91744</v>
+        <v>1.86969</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -1468,7 +1471,7 @@
         <v>43</v>
       </c>
       <c r="B84">
-        <v>1.86969</v>
+        <v>1.82194</v>
       </c>
     </row>
     <row r="85" spans="1:2">
@@ -1476,7 +1479,7 @@
         <v>43</v>
       </c>
       <c r="B85">
-        <v>1.86969</v>
+        <v>1.82194</v>
       </c>
     </row>
     <row r="86" spans="1:2">
@@ -1484,7 +1487,7 @@
         <v>44</v>
       </c>
       <c r="B86">
-        <v>1.82194</v>
+        <v>2.10844</v>
       </c>
     </row>
     <row r="87" spans="1:2">
@@ -1492,7 +1495,7 @@
         <v>44</v>
       </c>
       <c r="B87">
-        <v>1.82194</v>
+        <v>2.10844</v>
       </c>
     </row>
     <row r="88" spans="1:2">
@@ -1644,7 +1647,7 @@
         <v>54</v>
       </c>
       <c r="B106">
-        <v>1.798065</v>
+        <v>1.67869</v>
       </c>
     </row>
     <row r="107" spans="1:2">
@@ -1652,7 +1655,7 @@
         <v>54</v>
       </c>
       <c r="B107">
-        <v>1.798065</v>
+        <v>1.67869</v>
       </c>
     </row>
     <row r="108" spans="1:2">
@@ -1660,7 +1663,7 @@
         <v>55</v>
       </c>
       <c r="B108">
-        <v>1.67869</v>
+        <v>1.607065</v>
       </c>
     </row>
     <row r="109" spans="1:2">
@@ -1668,7 +1671,7 @@
         <v>55</v>
       </c>
       <c r="B109">
-        <v>1.67869</v>
+        <v>1.607065</v>
       </c>
     </row>
     <row r="110" spans="1:2">
@@ -1676,7 +1679,7 @@
         <v>56</v>
       </c>
       <c r="B110">
-        <v>1.607065</v>
+        <v>1.798065</v>
       </c>
     </row>
     <row r="111" spans="1:2">
@@ -1684,7 +1687,7 @@
         <v>56</v>
       </c>
       <c r="B111">
-        <v>1.607065</v>
+        <v>1.798065</v>
       </c>
     </row>
     <row r="112" spans="1:2">
@@ -1980,7 +1983,7 @@
         <v>75</v>
       </c>
       <c r="B148">
-        <v>2.58594</v>
+        <v>2.29944</v>
       </c>
     </row>
     <row r="149" spans="1:2">
@@ -1988,7 +1991,7 @@
         <v>75</v>
       </c>
       <c r="B149">
-        <v>2.58594</v>
+        <v>2.29944</v>
       </c>
     </row>
     <row r="150" spans="1:2">
@@ -2012,7 +2015,7 @@
         <v>77</v>
       </c>
       <c r="B152">
-        <v>2.29944</v>
+        <v>2.275565</v>
       </c>
     </row>
     <row r="153" spans="1:2">
@@ -2020,7 +2023,7 @@
         <v>77</v>
       </c>
       <c r="B153">
-        <v>2.29944</v>
+        <v>2.275565</v>
       </c>
     </row>
     <row r="154" spans="1:2">
@@ -2028,7 +2031,7 @@
         <v>78</v>
       </c>
       <c r="B154">
-        <v>2.275565</v>
+        <v>2.15619</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -2036,7 +2039,7 @@
         <v>78</v>
       </c>
       <c r="B155">
-        <v>2.275565</v>
+        <v>2.15619</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -2060,7 +2063,7 @@
         <v>80</v>
       </c>
       <c r="B158">
-        <v>2.15619</v>
+        <v>2.275565</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -2068,7 +2071,7 @@
         <v>80</v>
       </c>
       <c r="B159">
-        <v>2.15619</v>
+        <v>2.275565</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -2076,7 +2079,7 @@
         <v>81</v>
       </c>
       <c r="B160">
-        <v>2.275565</v>
+        <v>2.180065</v>
       </c>
     </row>
     <row r="161" spans="1:2">
@@ -2084,7 +2087,7 @@
         <v>81</v>
       </c>
       <c r="B161">
-        <v>2.275565</v>
+        <v>2.180065</v>
       </c>
     </row>
     <row r="162" spans="1:2">
@@ -2092,7 +2095,7 @@
         <v>82</v>
       </c>
       <c r="B162">
-        <v>2.180065</v>
+        <v>2.58594</v>
       </c>
     </row>
     <row r="163" spans="1:2">
@@ -2100,7 +2103,7 @@
         <v>82</v>
       </c>
       <c r="B163">
-        <v>2.180065</v>
+        <v>2.58594</v>
       </c>
     </row>
     <row r="164" spans="1:2">
@@ -2428,7 +2431,7 @@
         <v>103</v>
       </c>
       <c r="B204">
-        <v>1.941315</v>
+        <v>1.893565</v>
       </c>
     </row>
     <row r="205" spans="1:2">
@@ -2436,7 +2439,7 @@
         <v>103</v>
       </c>
       <c r="B205">
-        <v>1.941315</v>
+        <v>1.893565</v>
       </c>
     </row>
     <row r="206" spans="1:2">
@@ -2444,7 +2447,7 @@
         <v>104</v>
       </c>
       <c r="B206">
-        <v>1.893565</v>
+        <v>1.86969</v>
       </c>
     </row>
     <row r="207" spans="1:2">
@@ -2452,7 +2455,7 @@
         <v>104</v>
       </c>
       <c r="B207">
-        <v>1.893565</v>
+        <v>1.86969</v>
       </c>
     </row>
     <row r="208" spans="1:2">
@@ -2460,7 +2463,7 @@
         <v>105</v>
       </c>
       <c r="B208">
-        <v>1.86969</v>
+        <v>1.941315</v>
       </c>
     </row>
     <row r="209" spans="1:2">
@@ -2468,7 +2471,7 @@
         <v>105</v>
       </c>
       <c r="B209">
-        <v>1.86969</v>
+        <v>1.941315</v>
       </c>
     </row>
     <row r="210" spans="1:2">
@@ -2492,7 +2495,7 @@
         <v>107</v>
       </c>
       <c r="B212">
-        <v>1.941315</v>
+        <v>1.86969</v>
       </c>
     </row>
     <row r="213" spans="1:2">
@@ -2500,7 +2503,7 @@
         <v>107</v>
       </c>
       <c r="B213">
-        <v>1.941315</v>
+        <v>1.86969</v>
       </c>
     </row>
     <row r="214" spans="1:2">
@@ -2508,7 +2511,7 @@
         <v>108</v>
       </c>
       <c r="B214">
-        <v>1.86969</v>
+        <v>1.91744</v>
       </c>
     </row>
     <row r="215" spans="1:2">
@@ -2516,7 +2519,7 @@
         <v>108</v>
       </c>
       <c r="B215">
-        <v>1.86969</v>
+        <v>1.91744</v>
       </c>
     </row>
     <row r="216" spans="1:2">
@@ -2540,7 +2543,7 @@
         <v>110</v>
       </c>
       <c r="B218">
-        <v>1.91744</v>
+        <v>1.941315</v>
       </c>
     </row>
     <row r="219" spans="1:2">
@@ -2548,7 +2551,7 @@
         <v>110</v>
       </c>
       <c r="B219">
-        <v>1.91744</v>
+        <v>1.941315</v>
       </c>
     </row>
     <row r="220" spans="1:2">
@@ -2700,7 +2703,7 @@
         <v>120</v>
       </c>
       <c r="B238">
-        <v>1.654815</v>
+        <v>1.845815</v>
       </c>
     </row>
     <row r="239" spans="1:2">
@@ -2708,7 +2711,7 @@
         <v>120</v>
       </c>
       <c r="B239">
-        <v>1.654815</v>
+        <v>1.845815</v>
       </c>
     </row>
     <row r="240" spans="1:2">
@@ -2716,7 +2719,7 @@
         <v>121</v>
       </c>
       <c r="B240">
-        <v>1.845815</v>
+        <v>1.654815</v>
       </c>
     </row>
     <row r="241" spans="1:2">
@@ -2724,7 +2727,7 @@
         <v>121</v>
       </c>
       <c r="B241">
-        <v>1.845815</v>
+        <v>1.654815</v>
       </c>
     </row>
     <row r="242" spans="1:2">
@@ -2873,7 +2876,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -2958,7 +2961,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>809</v>
@@ -2966,7 +2969,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>809</v>
@@ -3262,7 +3265,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B50">
         <v>395.6</v>
@@ -3270,7 +3273,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B51">
         <v>395.6</v>
@@ -3278,7 +3281,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B52">
         <v>395.6</v>
@@ -3286,7 +3289,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B53">
         <v>395.6</v>
@@ -3294,7 +3297,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B54">
         <v>395.6</v>
@@ -3302,7 +3305,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B55">
         <v>395.6</v>
@@ -3310,7 +3313,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B56">
         <v>395.6</v>
@@ -3318,7 +3321,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B57">
         <v>395.6</v>
@@ -3326,7 +3329,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B58">
         <v>395.6</v>
@@ -3334,7 +3337,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B59">
         <v>395.6</v>
@@ -3342,7 +3345,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B60">
         <v>395.6</v>
@@ -3350,7 +3353,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B61">
         <v>395.6</v>
@@ -3358,7 +3361,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B62">
         <v>395.6</v>
@@ -3366,7 +3369,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B63">
         <v>395.6</v>
@@ -3374,7 +3377,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B64">
         <v>395.6</v>
@@ -3382,7 +3385,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B65">
         <v>395.6</v>
@@ -3390,7 +3393,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B66">
         <v>395.6</v>
@@ -3398,7 +3401,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B67">
         <v>395.6</v>
@@ -3406,7 +3409,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B68">
         <v>395.6</v>
@@ -3414,7 +3417,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B69">
         <v>395.6</v>
@@ -3505,7 +3508,7 @@
         <v>43</v>
       </c>
       <c r="B80">
-        <v>693.6</v>
+        <v>693.8</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -3513,7 +3516,7 @@
         <v>43</v>
       </c>
       <c r="B81">
-        <v>693.6</v>
+        <v>693.8</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -3521,7 +3524,7 @@
         <v>44</v>
       </c>
       <c r="B82">
-        <v>693.8</v>
+        <v>693.6</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -3529,7 +3532,7 @@
         <v>44</v>
       </c>
       <c r="B83">
-        <v>693.8</v>
+        <v>693.6</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -4017,7 +4020,7 @@
         <v>75</v>
       </c>
       <c r="B144">
-        <v>319</v>
+        <v>319.2</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -4025,7 +4028,7 @@
         <v>75</v>
       </c>
       <c r="B145">
-        <v>319</v>
+        <v>319.2</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -4097,7 +4100,7 @@
         <v>80</v>
       </c>
       <c r="B154">
-        <v>319.2</v>
+        <v>327.8</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -4105,7 +4108,7 @@
         <v>80</v>
       </c>
       <c r="B155">
-        <v>319.2</v>
+        <v>327.8</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -4113,7 +4116,7 @@
         <v>81</v>
       </c>
       <c r="B156">
-        <v>327.8</v>
+        <v>341.8</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -4121,7 +4124,7 @@
         <v>81</v>
       </c>
       <c r="B157">
-        <v>327.8</v>
+        <v>341.8</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -4129,7 +4132,7 @@
         <v>82</v>
       </c>
       <c r="B158">
-        <v>341.8</v>
+        <v>319</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -4137,7 +4140,7 @@
         <v>82</v>
       </c>
       <c r="B159">
-        <v>341.8</v>
+        <v>319</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -4734,7 +4737,7 @@
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B234">
         <v>352.8</v>
@@ -4742,7 +4745,7 @@
     </row>
     <row r="235" spans="1:2">
       <c r="A235" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B235">
         <v>352.8</v>
@@ -4894,7 +4897,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -4979,7 +4982,7 @@
     </row>
     <row r="12" spans="1:2">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B12">
         <v>809</v>
@@ -4987,7 +4990,7 @@
     </row>
     <row r="13" spans="1:2">
       <c r="A13" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B13">
         <v>809</v>
@@ -5283,7 +5286,7 @@
     </row>
     <row r="50" spans="1:2">
       <c r="A50" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B50">
         <v>395.6</v>
@@ -5291,7 +5294,7 @@
     </row>
     <row r="51" spans="1:2">
       <c r="A51" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B51">
         <v>395.6</v>
@@ -5299,7 +5302,7 @@
     </row>
     <row r="52" spans="1:2">
       <c r="A52" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B52">
         <v>395.6</v>
@@ -5307,7 +5310,7 @@
     </row>
     <row r="53" spans="1:2">
       <c r="A53" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B53">
         <v>395.6</v>
@@ -5315,7 +5318,7 @@
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B54">
         <v>395.6</v>
@@ -5323,7 +5326,7 @@
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B55">
         <v>395.6</v>
@@ -5331,7 +5334,7 @@
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B56">
         <v>395.6</v>
@@ -5339,7 +5342,7 @@
     </row>
     <row r="57" spans="1:2">
       <c r="A57" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B57">
         <v>395.6</v>
@@ -5347,7 +5350,7 @@
     </row>
     <row r="58" spans="1:2">
       <c r="A58" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B58">
         <v>395.6</v>
@@ -5355,7 +5358,7 @@
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B59">
         <v>395.6</v>
@@ -5363,7 +5366,7 @@
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B60">
         <v>395.6</v>
@@ -5371,7 +5374,7 @@
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="1" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B61">
         <v>395.6</v>
@@ -5379,7 +5382,7 @@
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B62">
         <v>395.6</v>
@@ -5387,7 +5390,7 @@
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="1" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B63">
         <v>395.6</v>
@@ -5395,7 +5398,7 @@
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B64">
         <v>395.6</v>
@@ -5403,7 +5406,7 @@
     </row>
     <row r="65" spans="1:2">
       <c r="A65" s="1" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B65">
         <v>395.6</v>
@@ -5411,7 +5414,7 @@
     </row>
     <row r="66" spans="1:2">
       <c r="A66" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B66">
         <v>395.6</v>
@@ -5419,7 +5422,7 @@
     </row>
     <row r="67" spans="1:2">
       <c r="A67" s="1" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B67">
         <v>395.6</v>
@@ -5427,7 +5430,7 @@
     </row>
     <row r="68" spans="1:2">
       <c r="A68" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B68">
         <v>395.6</v>
@@ -5435,7 +5438,7 @@
     </row>
     <row r="69" spans="1:2">
       <c r="A69" s="1" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B69">
         <v>395.6</v>
@@ -5526,7 +5529,7 @@
         <v>43</v>
       </c>
       <c r="B80">
-        <v>693.6</v>
+        <v>693.8</v>
       </c>
     </row>
     <row r="81" spans="1:2">
@@ -5534,7 +5537,7 @@
         <v>43</v>
       </c>
       <c r="B81">
-        <v>693.6</v>
+        <v>693.8</v>
       </c>
     </row>
     <row r="82" spans="1:2">
@@ -5542,7 +5545,7 @@
         <v>44</v>
       </c>
       <c r="B82">
-        <v>693.8</v>
+        <v>693.6</v>
       </c>
     </row>
     <row r="83" spans="1:2">
@@ -5550,7 +5553,7 @@
         <v>44</v>
       </c>
       <c r="B83">
-        <v>693.8</v>
+        <v>693.6</v>
       </c>
     </row>
     <row r="84" spans="1:2">
@@ -6038,7 +6041,7 @@
         <v>75</v>
       </c>
       <c r="B144">
-        <v>319</v>
+        <v>319.2</v>
       </c>
     </row>
     <row r="145" spans="1:2">
@@ -6046,7 +6049,7 @@
         <v>75</v>
       </c>
       <c r="B145">
-        <v>319</v>
+        <v>319.2</v>
       </c>
     </row>
     <row r="146" spans="1:2">
@@ -6118,7 +6121,7 @@
         <v>80</v>
       </c>
       <c r="B154">
-        <v>319.2</v>
+        <v>327.8</v>
       </c>
     </row>
     <row r="155" spans="1:2">
@@ -6126,7 +6129,7 @@
         <v>80</v>
       </c>
       <c r="B155">
-        <v>319.2</v>
+        <v>327.8</v>
       </c>
     </row>
     <row r="156" spans="1:2">
@@ -6134,7 +6137,7 @@
         <v>81</v>
       </c>
       <c r="B156">
-        <v>327.8</v>
+        <v>341.8</v>
       </c>
     </row>
     <row r="157" spans="1:2">
@@ -6142,7 +6145,7 @@
         <v>81</v>
       </c>
       <c r="B157">
-        <v>327.8</v>
+        <v>341.8</v>
       </c>
     </row>
     <row r="158" spans="1:2">
@@ -6150,7 +6153,7 @@
         <v>82</v>
       </c>
       <c r="B158">
-        <v>341.8</v>
+        <v>319</v>
       </c>
     </row>
     <row r="159" spans="1:2">
@@ -6158,7 +6161,7 @@
         <v>82</v>
       </c>
       <c r="B159">
-        <v>341.8</v>
+        <v>319</v>
       </c>
     </row>
     <row r="160" spans="1:2">
@@ -6755,7 +6758,7 @@
     </row>
     <row r="234" spans="1:2">
       <c r="A234" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B234">
         <v>352.8</v>
@@ -6763,7 +6766,7 @@
     </row>
     <row r="235" spans="1:2">
       <c r="A235" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B235">
         <v>352.8</v>

</xml_diff>